<commit_message>
actualización de tabla champion
</commit_message>
<xml_diff>
--- a/data/output/tables/champion_models.xlsx
+++ b/data/output/tables/champion_models.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>model</t>
   </si>
@@ -23,6 +23,27 @@
   </si>
   <si>
     <t>test_rmse</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>consumo_privado</t>
+  </si>
+  <si>
+    <t>exportaciones</t>
+  </si>
+  <si>
+    <t>gasto_publico</t>
+  </si>
+  <si>
+    <t>importaciones</t>
+  </si>
+  <si>
+    <t>inversiones</t>
+  </si>
+  <si>
+    <t>variacion</t>
   </si>
   <si>
     <t>lr</t>
@@ -386,86 +407,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
         <v>2052.214393768477</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2513.108597020475</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
         <v>13.154549082672</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2275.445492660668</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
         <v>2407.003495450783</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>15190.08447547815</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>235.1036593763999</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>3383.920983241372</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
         <v>0.2701928035102283</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>1522.486746418784</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
         <v>1255.879226075102</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>3105.390023382689</v>
       </c>
     </row>

</xml_diff>